<commit_message>
Modified auditbeatquery.py to fetch atleast 100K rows + time related code additions to gammarf.py file
</commit_message>
<xml_diff>
--- a/time_taken.xlsx
+++ b/time_taken.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Time Taken(mins)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>gamma</t>
   </si>
@@ -39,13 +36,31 @@
   </si>
   <si>
     <t>Rows</t>
+  </si>
+  <si>
+    <t>auditbeatquery</t>
+  </si>
+  <si>
+    <t>No.of Loops Required to Fetch the data</t>
+  </si>
+  <si>
+    <t>Total Time Taken(mins)</t>
+  </si>
+  <si>
+    <t>Time to save data</t>
+  </si>
+  <si>
+    <t>Time to Fetch data</t>
+  </si>
+  <si>
+    <t>in Minutes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,13 +68,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,13 +116,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,37 +422,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C3" s="1">
+        <v>523046</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.5798487186431798</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.388001199563344</v>
+      </c>
+      <c r="F3" s="1">
+        <f>D3-E3</f>
+        <v>4.1918475190798361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>8.3330000000000002</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>523046</v>
+      <c r="C4" s="1">
+        <v>110425</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.9470000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <f>0.0167811671892801+0.0101068019866943+0.00932354927062988+0.0110263029734293+0.0192538817723592</f>
+        <v>6.6491703192392781E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>D4-E4</f>
+        <v>2.8805082968076072</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
domoticz.py - added code to pull min 100K records
</commit_message>
<xml_diff>
--- a/time_taken.xlsx
+++ b/time_taken.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>gamma</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>in Minutes</t>
+  </si>
+  <si>
+    <t>domoticz</t>
   </si>
 </sst>
 </file>
@@ -134,10 +137,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,13 +442,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -461,7 +464,7 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -486,7 +489,7 @@
         <v>4.1918475190798361</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -506,6 +509,27 @@
       <c r="F4" s="1">
         <f>D4-E4</f>
         <v>2.8805082968076072</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100760</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.57740000000000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="F5" s="1">
+        <f>D5-E5</f>
+        <v>0.56830000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>